<commit_message>
Variable rates of gauge widening
The rate of yearly gauge widening is no more constant. Also, sensitivity analysis is now included for both gauge widening and renewal costs
</commit_message>
<xml_diff>
--- a/räls_livslängd/Wear/mistra_results_artificial.xlsx
+++ b/räls_livslängd/Wear/mistra_results_artificial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\mistra-inframaint\räls_livslängd\Wear\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C978B350-D447-4124-85D4-D852174DD66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A46308-13EC-440D-89D1-420A33E527DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{A70CFB27-6833-4726-9602-4BDAA622249F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A70CFB27-6833-4726-9602-4BDAA622249F}"/>
   </bookViews>
   <sheets>
     <sheet name="Wear" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="75">
   <si>
     <t>month 1</t>
   </si>
@@ -249,6 +249,21 @@
   </si>
   <si>
     <t>RCF residual (high rail)</t>
+  </si>
+  <si>
+    <t>extrapolation</t>
+  </si>
+  <si>
+    <t>grinding once</t>
+  </si>
+  <si>
+    <t>twice</t>
+  </si>
+  <si>
+    <t>3 times</t>
+  </si>
+  <si>
+    <t>once</t>
   </si>
 </sst>
 </file>
@@ -257,7 +272,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -315,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +364,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -366,7 +393,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -378,11 +405,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -1700,7 +1729,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B277D25-6310-4763-A9A3-46E6FFF4FD45}">
   <dimension ref="A5:AB40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3377,7 +3408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575556C3-9CD1-4D3F-93A7-9FEC3F5A934D}">
   <dimension ref="A5:AB39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3739,7 +3772,7 @@
       <c r="I11">
         <v>0.42220000000000002</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="9">
         <v>0.57210000000000005</v>
       </c>
       <c r="K11">
@@ -3828,7 +3861,7 @@
       <c r="L12">
         <v>1.3346</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="17">
         <v>1.5916999999999999</v>
       </c>
       <c r="P12" t="s">
@@ -4191,6 +4224,36 @@
       </c>
       <c r="AB19">
         <v>1.5158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>71</v>
+      </c>
+      <c r="N21" t="s">
+        <v>72</v>
+      </c>
+      <c r="O21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22">
+        <f>J9-J29</f>
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="M22" s="17">
+        <f>M12-M32</f>
+        <v>0.59169999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <f>M9-M29</f>
+        <v>0.1613</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -4371,22 +4434,22 @@
       <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="5">
-        <v>0</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
@@ -4396,16 +4459,16 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="M29">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="P29" t="s">
         <v>12</v>
@@ -4451,22 +4514,22 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="5">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
@@ -4476,16 +4539,16 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="P30" t="s">
         <v>13</v>
@@ -4531,41 +4594,41 @@
       <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="5">
-        <v>0</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0</v>
-      </c>
-      <c r="D31" s="5">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5">
-        <v>0</v>
-      </c>
-      <c r="F31" s="5">
-        <v>0</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>0.17</v>
       </c>
-      <c r="K31">
+      <c r="E31">
         <v>0.21</v>
       </c>
-      <c r="L31">
+      <c r="F31">
         <v>0.3</v>
       </c>
-      <c r="M31">
+      <c r="G31">
         <v>0.32</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="P31" t="s">
         <v>14</v>
@@ -4611,40 +4674,40 @@
       <c r="A32" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="5">
-        <v>0</v>
-      </c>
-      <c r="C32" s="5">
-        <v>0</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
         <v>0.11</v>
       </c>
-      <c r="J32">
+      <c r="D32">
         <v>0.46</v>
       </c>
-      <c r="K32">
+      <c r="E32">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L32">
+      <c r="F32">
         <v>0.77</v>
       </c>
-      <c r="M32">
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32" s="17">
         <v>1</v>
       </c>
       <c r="P32" t="s">
@@ -5035,8 +5098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C240127D-17EB-4812-A2BA-3FDC0D42802F}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5626,6 +5689,12 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="G19" s="9" t="s">
         <v>63</v>
       </c>
@@ -5665,7 +5734,9 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
       <c r="D22" t="s">
         <v>54</v>
       </c>
@@ -5680,7 +5751,9 @@
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
       <c r="D23" t="s">
         <v>54</v>
       </c>
@@ -5695,7 +5768,9 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
       <c r="D24" t="s">
         <v>54</v>
       </c>
@@ -5806,17 +5881,19 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33">
         <v>12</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="H33" s="15" t="s">
+      <c r="C33" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="H33" t="s">
         <v>46</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I33" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5869,9 +5946,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="B43" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final tests for VSD paper
</commit_message>
<xml_diff>
--- a/räls_livslängd/Wear/mistra_results_artificial.xlsx
+++ b/räls_livslängd/Wear/mistra_results_artificial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\mistra-inframaint\räls_livslängd\Wear\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A46308-13EC-440D-89D1-420A33E527DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C6B44C-B7C3-4388-B5A6-605CDE28F07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A70CFB27-6833-4726-9602-4BDAA622249F}"/>
+    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A70CFB27-6833-4726-9602-4BDAA622249F}"/>
   </bookViews>
   <sheets>
     <sheet name="Wear" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="78">
   <si>
     <t>month 1</t>
   </si>
@@ -260,10 +260,19 @@
     <t>twice</t>
   </si>
   <si>
-    <t>3 times</t>
-  </si>
-  <si>
     <t>once</t>
+  </si>
+  <si>
+    <t>.5</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -377,12 +386,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -410,8 +430,8 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -1729,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B277D25-6310-4763-A9A3-46E6FFF4FD45}">
   <dimension ref="A5:AB40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,8 +3428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575556C3-9CD1-4D3F-93A7-9FEC3F5A934D}">
   <dimension ref="A5:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,7 +3881,7 @@
       <c r="L12">
         <v>1.3346</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="16">
         <v>1.5916999999999999</v>
       </c>
       <c r="P12" t="s">
@@ -4227,33 +4247,46 @@
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E21" s="17">
+        <v>0.45500000000000002</v>
+      </c>
       <c r="M21" t="s">
         <v>71</v>
       </c>
       <c r="N21" t="s">
         <v>72</v>
       </c>
-      <c r="O21" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J22">
         <f>J9-J29</f>
         <v>0.13689999999999999</v>
       </c>
-      <c r="M22" s="17">
+      <c r="L22" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" s="16">
         <f>M12-M32</f>
         <v>0.59169999999999989</v>
       </c>
+      <c r="Q22" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>76</v>
+      </c>
       <c r="M23">
         <f>M9-M29</f>
         <v>0.1613</v>
+      </c>
+      <c r="O23">
+        <f>M32-M22</f>
+        <v>0.40830000000000011</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -4612,22 +4645,22 @@
       <c r="G31">
         <v>0.32</v>
       </c>
-      <c r="H31" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="H31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" t="s">
         <v>70</v>
       </c>
       <c r="J31" s="9">
         <v>0.5</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" t="s">
         <v>70</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L31" t="s">
         <v>70</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="M31" t="s">
         <v>70</v>
       </c>
       <c r="P31" t="s">
@@ -4692,22 +4725,22 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" t="s">
         <v>70</v>
       </c>
-      <c r="I32" s="16" t="s">
+      <c r="I32" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="16" t="s">
+      <c r="J32" t="s">
         <v>70</v>
       </c>
-      <c r="K32" s="16" t="s">
+      <c r="K32" t="s">
         <v>70</v>
       </c>
-      <c r="L32" s="16" t="s">
+      <c r="L32" t="s">
         <v>70</v>
       </c>
-      <c r="M32" s="17">
+      <c r="M32" s="16">
         <v>1</v>
       </c>
       <c r="P32" t="s">
@@ -5098,8 +5131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C240127D-17EB-4812-A2BA-3FDC0D42802F}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>